<commit_message>
added randomness to inventory holding costs in each region
</commit_message>
<xml_diff>
--- a/CostOfSales.xlsx
+++ b/CostOfSales.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/virginiamaguire/Documents/Optimization/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/virginiamaguire/Documents/Optimization/Project/15.093_optimization_methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC5C1E1-D370-1A42-BC61-50B9FF6B16B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F59AE85-961A-A94D-8DEF-59D71B61A673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="10620" windowHeight="17240" xr2:uid="{B8962302-2010-6343-8D48-89281927FE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,19 +36,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Year</t>
   </si>
   <si>
     <t>Cost of Sales (M)</t>
   </si>
+  <si>
+    <t>% of Revenue from shoes</t>
+  </si>
+  <si>
+    <t>Shoes - Cost of Sales ($M)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,14 +91,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,84 +416,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AAD8EE-8722-2647-9C59-D96264B0494E}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2023</v>
       </c>
       <c r="B2">
         <v>28925</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="1">
+        <v>0.68032029565753005</v>
+      </c>
+      <c r="D2" s="2">
+        <f>B2*C2</f>
+        <v>19678.264551894055</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2022</v>
       </c>
       <c r="B3">
         <v>25231</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="1">
+        <v>0.65735101727793566</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
+        <v>16585.623516939595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
       <c r="B4">
         <v>25576</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1">
+        <v>0.66293650042585406</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>16955.263934891642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2020</v>
       </c>
       <c r="B5">
         <v>21162</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="1">
+        <v>0.65577691485170808</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>13877.551072091846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2019</v>
       </c>
       <c r="B6">
         <v>21643</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="1">
+        <v>0.65154938670109752</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>14101.483376371854</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2018</v>
       </c>
       <c r="B7">
         <v>20441</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="1">
+        <v>0.64738203913131964</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>13233.136261883305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2017</v>
       </c>
       <c r="B8">
         <v>19038</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="1">
+        <v>0.65550373134328355</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>12479.480037313433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2016</v>
       </c>
       <c r="B9">
         <v>17405</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.65292107511336006</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>11364.091312348031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>